<commit_message>
Added results of runtime monitor and patch
</commit_message>
<xml_diff>
--- a/experiments/Consolidated Results from different techniques.xlsx
+++ b/experiments/Consolidated Results from different techniques.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgopinat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgopinat\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD77AC6-B9D2-44E1-A0F8-03D2613CEF5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A7B910-E2FA-4540-9D47-7DE00022CEC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{6E851A2A-318E-4F15-AEB0-BD2CB026064A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{6E851A2A-318E-4F15-AEB0-BD2CB026064A}"/>
   </bookViews>
   <sheets>
     <sheet name="Pattern-Train" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Mutation-Train" sheetId="12" r:id="rId3"/>
     <sheet name="Mutation-Test" sheetId="13" r:id="rId4"/>
     <sheet name="Last-Layer" sheetId="14" r:id="rId5"/>
-    <sheet name="Summary" sheetId="11" r:id="rId6"/>
+    <sheet name="Runtime-Monitor_Patch" sheetId="15" r:id="rId6"/>
+    <sheet name="Summary" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="93">
   <si>
     <t>LABEL 7</t>
   </si>
@@ -240,12 +241,94 @@
   <si>
     <t>Mutation Based Repair - Tarantula Localization using Poisoned Train_Set (only 600 poisoned inputs)</t>
   </si>
+  <si>
+    <t>POISONED</t>
+  </si>
+  <si>
+    <t>p: first 600 poisoned-mnist-train
+u: remaining poisoned-mnist-train
+P`: poisoned-mnist-test
+U`:mnist-test</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>p+u</t>
+  </si>
+  <si>
+    <t>P`</t>
+  </si>
+  <si>
+    <t>U`</t>
+  </si>
+  <si>
+    <t>Mis-classificationPattern, Guided, No Experts</t>
+  </si>
+  <si>
+    <t>Tunable Params</t>
+  </si>
+  <si>
+    <t>Evaluation Methodology</t>
+  </si>
+  <si>
+    <t>increase</t>
+  </si>
+  <si>
+    <t>avg increase</t>
+  </si>
+  <si>
+    <t>switch-off all neurons in pattern</t>
+  </si>
+  <si>
+    <t>flip all neuron activations in pattern</t>
+  </si>
+  <si>
+    <t>Coverage, Guided, No Experts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">increase </t>
+  </si>
+  <si>
+    <t>switch-off all top 20 neuron acts</t>
+  </si>
+  <si>
+    <t>flip all top 20 neuron acts</t>
+  </si>
+  <si>
+    <t>switch-off any of the top 20 neuron acts</t>
+  </si>
+  <si>
+    <t>flip any of the top 20 neuron acts</t>
+  </si>
+  <si>
+    <t>LOW-QUALITY</t>
+  </si>
+  <si>
+    <t>Train: mnist-train
+Test:mnist-test</t>
+  </si>
+  <si>
+    <t>None mis-classification pattern found</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>LABEL0:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,8 +412,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,8 +446,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -364,11 +461,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -480,6 +592,40 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4170,7 +4316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D12D6A94-C3A6-4756-A633-01A8292168B5}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
@@ -7280,11 +7426,735 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C066518F-A604-491F-8ED5-258FF25079BB}">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+    </row>
+    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50">
+        <v>10.3333333333333</v>
+      </c>
+      <c r="D4" s="50">
+        <v>99.883799999999994</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50">
+        <v>98.988333333333301</v>
+      </c>
+      <c r="G4" s="50">
+        <v>10.38</v>
+      </c>
+      <c r="H4" s="50">
+        <v>98.63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="55"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="56"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="57"/>
+      <c r="B7" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="57">
+        <f>(10.5-C4)</f>
+        <v>0.16666666666669983</v>
+      </c>
+      <c r="D7" s="57">
+        <f>(99.8838-D4)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="58">
+        <f>(C7+D7)/2</f>
+        <v>8.3333333333349913E-2</v>
+      </c>
+      <c r="F7" s="58">
+        <f>(98.99-F4)</f>
+        <v>1.6666666666935726E-3</v>
+      </c>
+      <c r="G7" s="58">
+        <v>10.94</v>
+      </c>
+      <c r="H7" s="59">
+        <v>98.63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="50">
+        <f>(10.333-C4)</f>
+        <v>-3.3333333329998993E-4</v>
+      </c>
+      <c r="D8" s="50">
+        <f>(99.8838-D4)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="57">
+        <f>(C8+D8)/2</f>
+        <v>-1.6666666664999497E-4</v>
+      </c>
+      <c r="F8" s="50">
+        <f>(98.9833-F4)</f>
+        <v>-5.0333333333014707E-3</v>
+      </c>
+      <c r="G8" s="50">
+        <v>11.1</v>
+      </c>
+      <c r="H8" s="48">
+        <v>98.63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="55"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="56"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="48"/>
+      <c r="B11" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="57">
+        <f>(10.8333-C4)</f>
+        <v>0.49996666666669931</v>
+      </c>
+      <c r="D11" s="57">
+        <f>(99.8838-D4)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="57">
+        <f>(C11+D11)/2</f>
+        <v>0.24998333333334966</v>
+      </c>
+      <c r="F11" s="48">
+        <f>(98.9933-F4)</f>
+        <v>4.9666666667036452E-3</v>
+      </c>
+      <c r="G11" s="48">
+        <v>10.76</v>
+      </c>
+      <c r="H11" s="57">
+        <v>98.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="48"/>
+      <c r="B12" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="50">
+        <f>(11.1666-C4)</f>
+        <v>0.83326666666670057</v>
+      </c>
+      <c r="D12" s="50">
+        <f>(99.8838-D4)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="50">
+        <f>(C12+D12)/2</f>
+        <v>0.41663333333335029</v>
+      </c>
+      <c r="F12" s="48">
+        <f>(98.996-F4)</f>
+        <v>7.6666666666937999E-3</v>
+      </c>
+      <c r="G12" s="48">
+        <v>11.14</v>
+      </c>
+      <c r="H12" s="50">
+        <v>98.63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="48"/>
+      <c r="B13" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="48">
+        <f>(54.166-C4)</f>
+        <v>43.832666666666697</v>
+      </c>
+      <c r="D13" s="48">
+        <f>(98.3485-D4)</f>
+        <v>-1.5352999999999923</v>
+      </c>
+      <c r="E13" s="50">
+        <f t="shared" ref="E13:E14" si="0">(C13+D13)/2</f>
+        <v>21.148683333333352</v>
+      </c>
+      <c r="F13" s="48">
+        <f>(97.9066-F4)</f>
+        <v>-1.0817333333333039</v>
+      </c>
+      <c r="G13" s="48">
+        <v>58.609000000000002</v>
+      </c>
+      <c r="H13" s="48">
+        <v>96.87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="48"/>
+      <c r="B14" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="48">
+        <f>(65.5-C4)</f>
+        <v>55.1666666666667</v>
+      </c>
+      <c r="D14" s="48">
+        <f>(87.8958266695847-D4)</f>
+        <v>-11.987973330415301</v>
+      </c>
+      <c r="E14" s="51">
+        <f t="shared" si="0"/>
+        <v>21.5893466681257</v>
+      </c>
+      <c r="F14" s="48">
+        <f>(87.6733-F4)</f>
+        <v>-11.315033333333304</v>
+      </c>
+      <c r="G14" s="60">
+        <v>70.319999999999993</v>
+      </c>
+      <c r="H14" s="60">
+        <v>86.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+    </row>
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="49"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="51">
+        <v>96.578000000000003</v>
+      </c>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51">
+        <v>96.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" s="55"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="50"/>
+      <c r="B22" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" s="50"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="50"/>
+      <c r="B23" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="50"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="55"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="56"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="48"/>
+      <c r="B26" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="50"/>
+      <c r="F26" s="48">
+        <v>96.433000000000007</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" s="48">
+        <v>96.28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="48"/>
+      <c r="B27" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="50"/>
+      <c r="F27" s="48">
+        <v>89.51</v>
+      </c>
+      <c r="G27" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="48">
+        <v>89.63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="48"/>
+      <c r="B28" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="50"/>
+      <c r="F28" s="48">
+        <v>96.44</v>
+      </c>
+      <c r="G28" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="48">
+        <v>96.27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="48"/>
+      <c r="B29" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="50"/>
+      <c r="F29" s="48">
+        <v>88.656000000000006</v>
+      </c>
+      <c r="G29" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="48">
+        <v>88.73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="48"/>
+      <c r="B30" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="48"/>
+      <c r="H30" s="51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="48"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51">
+        <v>98.918999999999997</v>
+      </c>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51">
+        <v>99.183000000000007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="48"/>
+      <c r="B32" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="50"/>
+      <c r="F32" s="48">
+        <v>97.433700000000002</v>
+      </c>
+      <c r="G32" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H32" s="48"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="48"/>
+      <c r="B33" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="50"/>
+      <c r="F33" s="48">
+        <v>88.552999999999997</v>
+      </c>
+      <c r="G33" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H33" s="48"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="48"/>
+      <c r="B34" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="50"/>
+      <c r="F34" s="48">
+        <v>95.17</v>
+      </c>
+      <c r="G34" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H34" s="48">
+        <v>95.816000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="48"/>
+      <c r="B35" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="50"/>
+      <c r="F35" s="48">
+        <v>54.88</v>
+      </c>
+      <c r="G35" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="48">
+        <v>54.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="G20:H20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7C8AE8-68EA-4CD1-89FD-4632DB72F050}">
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
results last layer added
</commit_message>
<xml_diff>
--- a/experiments/Consolidated Results from different techniques.xlsx
+++ b/experiments/Consolidated Results from different techniques.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgopinat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musman\Desktop\DNN-Repair\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A7B910-E2FA-4540-9D47-7DE00022CEC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C60D08-2288-4F7B-BB33-1C4C810C62A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{6E851A2A-318E-4F15-AEB0-BD2CB026064A}"/>
   </bookViews>
@@ -18,8 +18,9 @@
     <sheet name="Mutation-Train" sheetId="12" r:id="rId3"/>
     <sheet name="Mutation-Test" sheetId="13" r:id="rId4"/>
     <sheet name="Last-Layer" sheetId="14" r:id="rId5"/>
-    <sheet name="Runtime-Monitor_Patch" sheetId="15" r:id="rId6"/>
-    <sheet name="Summary" sheetId="11" r:id="rId7"/>
+    <sheet name="Last_Layer 5-21-2020" sheetId="16" r:id="rId6"/>
+    <sheet name="Runtime-Monitor_Patch" sheetId="15" r:id="rId7"/>
+    <sheet name="Summary" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="100">
   <si>
     <t>LABEL 7</t>
   </si>
@@ -323,6 +324,27 @@
   <si>
     <t>LABEL0:</t>
   </si>
+  <si>
+    <t>Train-Set</t>
+  </si>
+  <si>
+    <t>Test-Set</t>
+  </si>
+  <si>
+    <t>Poisoned Test-Set</t>
+  </si>
+  <si>
+    <t>Expert#</t>
+  </si>
+  <si>
+    <t>Pre-Repair</t>
+  </si>
+  <si>
+    <t>Post-Repair</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
 </sst>
 </file>
 
@@ -421,7 +443,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,6 +471,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -609,12 +637,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -626,6 +648,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6534,7 +6577,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7426,11 +7469,554 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9BC920C-48A2-4140-B7CF-8FF35C410D86}">
+  <dimension ref="A1:Q11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="61" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" style="61" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="61"/>
+    <col min="7" max="7" width="7.33203125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="61" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" style="61" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="61"/>
+    <col min="13" max="13" width="7.33203125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.77734375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" style="61" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.88671875" style="61" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C1" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="N2" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="63">
+        <v>0</v>
+      </c>
+      <c r="B3" s="64">
+        <v>98.970116495019397</v>
+      </c>
+      <c r="C3" s="64">
+        <v>99.93</v>
+      </c>
+      <c r="D3" s="65">
+        <f>SUM(C3-B3)</f>
+        <v>0.95988350498060981</v>
+      </c>
+      <c r="E3" s="64">
+        <v>98.45</v>
+      </c>
+      <c r="G3" s="63">
+        <v>0</v>
+      </c>
+      <c r="H3" s="64">
+        <v>99.387755102040799</v>
+      </c>
+      <c r="I3" s="64">
+        <v>99.897959183673393</v>
+      </c>
+      <c r="J3" s="65">
+        <f>SUM(I3-H3)</f>
+        <v>0.5102040816325939</v>
+      </c>
+      <c r="K3" s="64">
+        <v>98.04</v>
+      </c>
+      <c r="M3" s="63">
+        <v>0</v>
+      </c>
+      <c r="N3" s="64">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="O3" s="64">
+        <v>86.224489795918302</v>
+      </c>
+      <c r="P3" s="65">
+        <f>SUM(O3-N3)</f>
+        <v>86.122448979591766</v>
+      </c>
+      <c r="Q3" s="64">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="63">
+        <v>1</v>
+      </c>
+      <c r="B4" s="64">
+        <v>98.709581726490597</v>
+      </c>
+      <c r="C4" s="64">
+        <v>99.93</v>
+      </c>
+      <c r="D4" s="65">
+        <f t="shared" ref="D4:D11" si="0">SUM(C4-B4)</f>
+        <v>1.2204182735094093</v>
+      </c>
+      <c r="E4" s="64">
+        <v>95.078333333333305</v>
+      </c>
+      <c r="G4" s="63">
+        <v>1</v>
+      </c>
+      <c r="H4" s="64">
+        <v>99.4713656387665</v>
+      </c>
+      <c r="I4" s="64">
+        <v>99.7356828193832</v>
+      </c>
+      <c r="J4" s="65">
+        <f t="shared" ref="J4:J11" si="1">SUM(I4-H4)</f>
+        <v>0.2643171806167004</v>
+      </c>
+      <c r="K4" s="64">
+        <v>94.24</v>
+      </c>
+      <c r="M4" s="63">
+        <v>1</v>
+      </c>
+      <c r="N4" s="64">
+        <v>0</v>
+      </c>
+      <c r="O4" s="64">
+        <v>89.955947136563793</v>
+      </c>
+      <c r="P4" s="65">
+        <f t="shared" ref="P4:P11" si="2">SUM(O4-N4)</f>
+        <v>89.955947136563793</v>
+      </c>
+      <c r="Q4" s="64">
+        <v>20.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="63">
+        <v>2</v>
+      </c>
+      <c r="B5" s="64">
+        <v>98.774756629741503</v>
+      </c>
+      <c r="C5" s="64">
+        <v>99.28</v>
+      </c>
+      <c r="D5" s="65">
+        <f t="shared" si="0"/>
+        <v>0.50524337025849775</v>
+      </c>
+      <c r="E5" s="64">
+        <v>97.43</v>
+      </c>
+      <c r="G5" s="63">
+        <v>2</v>
+      </c>
+      <c r="H5" s="64">
+        <v>97.868217054263496</v>
+      </c>
+      <c r="I5" s="64">
+        <v>98.74</v>
+      </c>
+      <c r="J5" s="65">
+        <f t="shared" si="1"/>
+        <v>0.8717829457364985</v>
+      </c>
+      <c r="K5" s="64">
+        <v>97.12</v>
+      </c>
+      <c r="M5" s="63">
+        <v>2</v>
+      </c>
+      <c r="N5" s="64">
+        <v>0</v>
+      </c>
+      <c r="O5" s="64">
+        <v>78.290000000000006</v>
+      </c>
+      <c r="P5" s="65">
+        <f t="shared" si="2"/>
+        <v>78.290000000000006</v>
+      </c>
+      <c r="Q5" s="64">
+        <v>18.29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="63">
+        <v>3</v>
+      </c>
+      <c r="B6" s="64">
+        <v>98.956124612624293</v>
+      </c>
+      <c r="C6" s="64">
+        <v>99.84</v>
+      </c>
+      <c r="D6" s="65">
+        <f t="shared" si="0"/>
+        <v>0.88387538737570992</v>
+      </c>
+      <c r="E6" s="64">
+        <v>96.92</v>
+      </c>
+      <c r="G6" s="63">
+        <v>3</v>
+      </c>
+      <c r="H6" s="64">
+        <v>98.811881188118804</v>
+      </c>
+      <c r="I6" s="64">
+        <v>99.41</v>
+      </c>
+      <c r="J6" s="65">
+        <f t="shared" si="1"/>
+        <v>0.59811881188119287</v>
+      </c>
+      <c r="K6" s="64">
+        <v>96.55</v>
+      </c>
+      <c r="M6" s="63">
+        <v>3</v>
+      </c>
+      <c r="N6" s="64">
+        <v>0</v>
+      </c>
+      <c r="O6" s="64">
+        <v>73.27</v>
+      </c>
+      <c r="P6" s="65">
+        <f t="shared" si="2"/>
+        <v>73.27</v>
+      </c>
+      <c r="Q6" s="64">
+        <v>17.760000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="63">
+        <v>4</v>
+      </c>
+      <c r="B7" s="64">
+        <v>98.870249914412796</v>
+      </c>
+      <c r="C7" s="64">
+        <v>99.9</v>
+      </c>
+      <c r="D7" s="65">
+        <f t="shared" si="0"/>
+        <v>1.0297500855872102</v>
+      </c>
+      <c r="E7" s="64">
+        <v>97.13</v>
+      </c>
+      <c r="G7" s="63">
+        <v>4</v>
+      </c>
+      <c r="H7" s="64">
+        <v>98.778004073319707</v>
+      </c>
+      <c r="I7" s="64">
+        <v>99.389002036659804</v>
+      </c>
+      <c r="J7" s="65">
+        <f t="shared" si="1"/>
+        <v>0.61099796334009682</v>
+      </c>
+      <c r="K7" s="64">
+        <v>96.94</v>
+      </c>
+      <c r="M7" s="63">
+        <v>4</v>
+      </c>
+      <c r="N7" s="64">
+        <v>0.10183299389002</v>
+      </c>
+      <c r="O7" s="64">
+        <v>81.67</v>
+      </c>
+      <c r="P7" s="65">
+        <f t="shared" si="2"/>
+        <v>81.568167006109988</v>
+      </c>
+      <c r="Q7" s="64">
+        <v>18.149999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="63">
+        <v>5</v>
+      </c>
+      <c r="B8" s="64">
+        <v>98.985427042981001</v>
+      </c>
+      <c r="C8" s="64">
+        <v>99.87</v>
+      </c>
+      <c r="D8" s="65">
+        <f t="shared" si="0"/>
+        <v>0.88457295701900307</v>
+      </c>
+      <c r="E8" s="64">
+        <v>89.79</v>
+      </c>
+      <c r="G8" s="63">
+        <v>5</v>
+      </c>
+      <c r="H8" s="64">
+        <v>98.654708520179298</v>
+      </c>
+      <c r="I8" s="64">
+        <v>99.22</v>
+      </c>
+      <c r="J8" s="65">
+        <f t="shared" si="1"/>
+        <v>0.56529147982070072</v>
+      </c>
+      <c r="K8" s="64">
+        <v>90.34</v>
+      </c>
+      <c r="M8" s="63">
+        <v>5</v>
+      </c>
+      <c r="N8" s="64">
+        <v>0.112107623318385</v>
+      </c>
+      <c r="O8" s="64">
+        <v>90.69</v>
+      </c>
+      <c r="P8" s="65">
+        <f t="shared" si="2"/>
+        <v>90.577892376681618</v>
+      </c>
+      <c r="Q8" s="64">
+        <v>16.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="63">
+        <v>6</v>
+      </c>
+      <c r="B9" s="64">
+        <v>99.036836769178706</v>
+      </c>
+      <c r="C9" s="64">
+        <v>99.97</v>
+      </c>
+      <c r="D9" s="65">
+        <f t="shared" si="0"/>
+        <v>0.93316323082129315</v>
+      </c>
+      <c r="E9" s="64">
+        <v>96.3</v>
+      </c>
+      <c r="G9" s="63">
+        <v>6</v>
+      </c>
+      <c r="H9" s="64">
+        <v>98.643006263047994</v>
+      </c>
+      <c r="I9" s="64">
+        <v>99.06</v>
+      </c>
+      <c r="J9" s="65">
+        <f t="shared" si="1"/>
+        <v>0.41699373695200848</v>
+      </c>
+      <c r="K9" s="64">
+        <v>95.71</v>
+      </c>
+      <c r="M9" s="63">
+        <v>6</v>
+      </c>
+      <c r="N9" s="64">
+        <v>0.73068893528183698</v>
+      </c>
+      <c r="O9" s="64">
+        <v>98.23</v>
+      </c>
+      <c r="P9" s="65">
+        <f t="shared" si="2"/>
+        <v>97.499311064718171</v>
+      </c>
+      <c r="Q9" s="64">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="63">
+        <v>8</v>
+      </c>
+      <c r="B10" s="64">
+        <v>99.025807554264205</v>
+      </c>
+      <c r="C10" s="64">
+        <v>99.88</v>
+      </c>
+      <c r="D10" s="65">
+        <f t="shared" si="0"/>
+        <v>0.85419244573579078</v>
+      </c>
+      <c r="E10" s="64">
+        <v>94.17</v>
+      </c>
+      <c r="G10" s="63">
+        <v>8</v>
+      </c>
+      <c r="H10" s="64">
+        <v>98.665297741273093</v>
+      </c>
+      <c r="I10" s="64">
+        <v>99.49</v>
+      </c>
+      <c r="J10" s="65">
+        <f t="shared" si="1"/>
+        <v>0.8247022587269015</v>
+      </c>
+      <c r="K10" s="64">
+        <v>93.47</v>
+      </c>
+      <c r="M10" s="63">
+        <v>8</v>
+      </c>
+      <c r="N10" s="64">
+        <v>0</v>
+      </c>
+      <c r="O10" s="64">
+        <v>63.55</v>
+      </c>
+      <c r="P10" s="65">
+        <f t="shared" si="2"/>
+        <v>63.55</v>
+      </c>
+      <c r="Q10" s="64">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="63">
+        <v>9</v>
+      </c>
+      <c r="B11" s="64">
+        <v>98.554378887207903</v>
+      </c>
+      <c r="C11" s="64">
+        <v>99.92</v>
+      </c>
+      <c r="D11" s="65">
+        <f t="shared" si="0"/>
+        <v>1.3656211127920983</v>
+      </c>
+      <c r="E11" s="64">
+        <v>96.54</v>
+      </c>
+      <c r="G11" s="63">
+        <v>9</v>
+      </c>
+      <c r="H11" s="64">
+        <v>97.224975222992995</v>
+      </c>
+      <c r="I11" s="64">
+        <v>98.71</v>
+      </c>
+      <c r="J11" s="65">
+        <f t="shared" si="1"/>
+        <v>1.4850247770069984</v>
+      </c>
+      <c r="K11" s="64">
+        <v>96.38</v>
+      </c>
+      <c r="M11" s="63">
+        <v>9</v>
+      </c>
+      <c r="N11" s="64">
+        <v>0</v>
+      </c>
+      <c r="O11" s="64">
+        <v>93.06</v>
+      </c>
+      <c r="P11" s="65">
+        <f t="shared" si="2"/>
+        <v>93.06</v>
+      </c>
+      <c r="Q11" s="64">
+        <v>19.68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C066518F-A604-491F-8ED5-258FF25079BB}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7514,20 +8100,20 @@
       <c r="A5" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="54" t="s">
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="55"/>
+      <c r="H5" s="60"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="56"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51" t="s">
         <v>77</v>
@@ -7549,30 +8135,30 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="57"/>
-      <c r="B7" s="57" t="s">
+      <c r="A7" s="55"/>
+      <c r="B7" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="57">
+      <c r="C7" s="55">
         <f>(10.5-C4)</f>
         <v>0.16666666666669983</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="55">
         <f>(99.8838-D4)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="56">
         <f>(C7+D7)/2</f>
         <v>8.3333333333349913E-2</v>
       </c>
-      <c r="F7" s="58">
+      <c r="F7" s="56">
         <f>(98.99-F4)</f>
         <v>1.6666666666935726E-3</v>
       </c>
-      <c r="G7" s="58">
+      <c r="G7" s="56">
         <v>10.94</v>
       </c>
-      <c r="H7" s="59">
+      <c r="H7" s="57">
         <v>98.63</v>
       </c>
     </row>
@@ -7589,7 +8175,7 @@
         <f>(99.8838-D4)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="57">
+      <c r="E8" s="55">
         <f>(C8+D8)/2</f>
         <v>-1.6666666664999497E-4</v>
       </c>
@@ -7608,20 +8194,20 @@
       <c r="A9" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="54" t="s">
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="55"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="56"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51" t="s">
         <v>77</v>
@@ -7647,15 +8233,15 @@
       <c r="B11" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="57">
+      <c r="C11" s="55">
         <f>(10.8333-C4)</f>
         <v>0.49996666666669931</v>
       </c>
-      <c r="D11" s="57">
+      <c r="D11" s="55">
         <f>(99.8838-D4)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="57">
+      <c r="E11" s="55">
         <f>(C11+D11)/2</f>
         <v>0.24998333333334966</v>
       </c>
@@ -7666,7 +8252,7 @@
       <c r="G11" s="48">
         <v>10.76</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="55">
         <v>98.63</v>
       </c>
     </row>
@@ -7747,10 +8333,10 @@
         <f>(87.6733-F4)</f>
         <v>-11.315033333333304</v>
       </c>
-      <c r="G14" s="60">
+      <c r="G14" s="58">
         <v>70.319999999999993</v>
       </c>
-      <c r="H14" s="60">
+      <c r="H14" s="58">
         <v>86.53</v>
       </c>
     </row>
@@ -7822,20 +8408,20 @@
       <c r="A20" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="54" t="s">
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="H20" s="55"/>
+      <c r="H20" s="60"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="54" t="s">
         <v>89</v>
       </c>
       <c r="B21" s="51"/>
@@ -7896,20 +8482,20 @@
       <c r="A24" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="54" t="s">
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="H24" s="55"/>
+      <c r="H24" s="60"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="56"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="51"/>
       <c r="C25" s="51" t="s">
         <v>69</v>
@@ -8149,7 +8735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7C8AE8-68EA-4CD1-89FD-4632DB72F050}">
   <dimension ref="A1:U39"/>
   <sheetViews>

</xml_diff>

<commit_message>
combination results for last layer
</commit_message>
<xml_diff>
--- a/experiments/Consolidated Results from different techniques.xlsx
+++ b/experiments/Consolidated Results from different techniques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musman\Desktop\DNN-Repair\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DCDEB2-A58F-4B40-B055-D246448D62CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4C3688-B63A-408C-A6DE-3497945901D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{6E851A2A-318E-4F15-AEB0-BD2CB026064A}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="113">
   <si>
     <t>LABEL 7</t>
   </si>
@@ -350,18 +350,6 @@
     <t>Poisoned Model on Poisoned Test-Set</t>
   </si>
   <si>
-    <t>No Expert returned C</t>
-  </si>
-  <si>
-    <t>Expert C returned C</t>
-  </si>
-  <si>
-    <t>Multiple experts returned</t>
-  </si>
-  <si>
-    <t>Overall Accuracy - Expert Combined</t>
-  </si>
-  <si>
     <t>Low Quality Model on Train-set</t>
   </si>
   <si>
@@ -384,6 +372,18 @@
   </si>
   <si>
     <t>Accuracy for all inputs</t>
+  </si>
+  <si>
+    <t>Naïve</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+  <si>
+    <t>Vote</t>
+  </si>
+  <si>
+    <t>Precision</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -685,6 +685,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -698,12 +715,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7505,10 +7520,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9BC920C-48A2-4140-B7CF-8FF35C410D86}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7534,1050 +7549,1314 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65" t="s">
         <v>100</v>
       </c>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
     </row>
     <row r="2" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="F2" s="65"/>
+      <c r="G2" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="M2" s="46" t="s">
+      <c r="L2" s="65"/>
+      <c r="M2" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="N2" s="46" t="s">
+      <c r="N2" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="O2" s="46" t="s">
+      <c r="O2" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="P2" s="46" t="s">
+      <c r="P2" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="46" t="s">
+      <c r="Q2" s="66" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="60">
-        <v>0</v>
-      </c>
-      <c r="B3" s="61">
+      <c r="A3" s="67">
+        <v>0</v>
+      </c>
+      <c r="B3" s="68">
         <v>98.970116495019397</v>
       </c>
-      <c r="C3" s="61">
+      <c r="C3" s="68">
         <v>99.93</v>
       </c>
-      <c r="D3" s="62">
-        <f>SUM(C3-B3)</f>
+      <c r="D3" s="69">
         <v>0.95988350498060981</v>
       </c>
-      <c r="E3" s="61">
+      <c r="E3" s="68">
         <v>98.45</v>
       </c>
-      <c r="G3" s="60">
-        <v>0</v>
-      </c>
-      <c r="H3" s="61">
+      <c r="F3" s="63"/>
+      <c r="G3" s="67">
+        <v>0</v>
+      </c>
+      <c r="H3" s="68">
         <v>99.387755102040799</v>
       </c>
-      <c r="I3" s="61">
+      <c r="I3" s="68">
         <v>99.897959183673393</v>
       </c>
-      <c r="J3" s="62">
-        <f>SUM(I3-H3)</f>
+      <c r="J3" s="69">
         <v>0.5102040816325939</v>
       </c>
-      <c r="K3" s="61">
+      <c r="K3" s="68">
         <v>98.04</v>
       </c>
-      <c r="M3" s="60">
-        <v>0</v>
-      </c>
-      <c r="N3" s="61">
+      <c r="L3" s="63"/>
+      <c r="M3" s="67">
+        <v>0</v>
+      </c>
+      <c r="N3" s="68">
         <v>0.10204081632653</v>
       </c>
-      <c r="O3" s="61">
+      <c r="O3" s="68">
         <v>86.224489795918302</v>
       </c>
-      <c r="P3" s="62">
-        <f>SUM(O3-N3)</f>
+      <c r="P3" s="69">
         <v>86.122448979591766</v>
       </c>
-      <c r="Q3" s="61">
+      <c r="Q3" s="68">
         <v>18.75</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="60">
+      <c r="A4" s="67">
         <v>1</v>
       </c>
-      <c r="B4" s="61">
+      <c r="B4" s="68">
         <v>98.709581726490597</v>
       </c>
-      <c r="C4" s="61">
+      <c r="C4" s="68">
         <v>99.93</v>
       </c>
-      <c r="D4" s="62">
-        <f t="shared" ref="D4:D11" si="0">SUM(C4-B4)</f>
+      <c r="D4" s="69">
         <v>1.2204182735094093</v>
       </c>
-      <c r="E4" s="61">
+      <c r="E4" s="68">
         <v>95.078333333333305</v>
       </c>
-      <c r="G4" s="60">
+      <c r="F4" s="63"/>
+      <c r="G4" s="67">
         <v>1</v>
       </c>
-      <c r="H4" s="61">
+      <c r="H4" s="68">
         <v>99.4713656387665</v>
       </c>
-      <c r="I4" s="61">
+      <c r="I4" s="68">
         <v>99.7356828193832</v>
       </c>
-      <c r="J4" s="62">
-        <f t="shared" ref="J4:J11" si="1">SUM(I4-H4)</f>
+      <c r="J4" s="69">
         <v>0.2643171806167004</v>
       </c>
-      <c r="K4" s="61">
+      <c r="K4" s="68">
         <v>94.24</v>
       </c>
-      <c r="M4" s="60">
+      <c r="L4" s="63"/>
+      <c r="M4" s="67">
         <v>1</v>
       </c>
-      <c r="N4" s="61">
-        <v>0</v>
-      </c>
-      <c r="O4" s="61">
+      <c r="N4" s="68">
+        <v>0</v>
+      </c>
+      <c r="O4" s="68">
         <v>89.955947136563793</v>
       </c>
-      <c r="P4" s="62">
-        <f t="shared" ref="P4:P11" si="2">SUM(O4-N4)</f>
+      <c r="P4" s="69">
         <v>89.955947136563793</v>
       </c>
-      <c r="Q4" s="61">
+      <c r="Q4" s="68">
         <v>20.46</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="60">
+      <c r="A5" s="67">
         <v>2</v>
       </c>
-      <c r="B5" s="61">
+      <c r="B5" s="68">
         <v>98.774756629741503</v>
       </c>
-      <c r="C5" s="61">
+      <c r="C5" s="68">
         <v>99.28</v>
       </c>
-      <c r="D5" s="62">
-        <f t="shared" si="0"/>
+      <c r="D5" s="69">
         <v>0.50524337025849775</v>
       </c>
-      <c r="E5" s="61">
+      <c r="E5" s="68">
         <v>97.43</v>
       </c>
-      <c r="G5" s="60">
+      <c r="F5" s="63"/>
+      <c r="G5" s="67">
         <v>2</v>
       </c>
-      <c r="H5" s="61">
+      <c r="H5" s="68">
         <v>97.868217054263496</v>
       </c>
-      <c r="I5" s="61">
+      <c r="I5" s="68">
         <v>98.74</v>
       </c>
-      <c r="J5" s="62">
-        <f t="shared" si="1"/>
+      <c r="J5" s="69">
         <v>0.8717829457364985</v>
       </c>
-      <c r="K5" s="61">
+      <c r="K5" s="68">
         <v>97.12</v>
       </c>
-      <c r="M5" s="60">
+      <c r="L5" s="63"/>
+      <c r="M5" s="67">
         <v>2</v>
       </c>
-      <c r="N5" s="61">
-        <v>0</v>
-      </c>
-      <c r="O5" s="61">
+      <c r="N5" s="68">
+        <v>0</v>
+      </c>
+      <c r="O5" s="68">
         <v>78.290000000000006</v>
       </c>
-      <c r="P5" s="62">
-        <f t="shared" si="2"/>
+      <c r="P5" s="69">
         <v>78.290000000000006</v>
       </c>
-      <c r="Q5" s="61">
+      <c r="Q5" s="68">
         <v>18.29</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="60">
+      <c r="A6" s="67">
         <v>3</v>
       </c>
-      <c r="B6" s="61">
+      <c r="B6" s="68">
         <v>98.956124612624293</v>
       </c>
-      <c r="C6" s="61">
+      <c r="C6" s="68">
         <v>99.84</v>
       </c>
-      <c r="D6" s="62">
-        <f t="shared" si="0"/>
+      <c r="D6" s="69">
         <v>0.88387538737570992</v>
       </c>
-      <c r="E6" s="61">
+      <c r="E6" s="68">
         <v>96.92</v>
       </c>
-      <c r="G6" s="60">
+      <c r="F6" s="63"/>
+      <c r="G6" s="67">
         <v>3</v>
       </c>
-      <c r="H6" s="61">
+      <c r="H6" s="68">
         <v>98.811881188118804</v>
       </c>
-      <c r="I6" s="61">
+      <c r="I6" s="68">
         <v>99.41</v>
       </c>
-      <c r="J6" s="62">
-        <f t="shared" si="1"/>
+      <c r="J6" s="69">
         <v>0.59811881188119287</v>
       </c>
-      <c r="K6" s="61">
+      <c r="K6" s="68">
         <v>96.55</v>
       </c>
-      <c r="M6" s="60">
+      <c r="L6" s="63"/>
+      <c r="M6" s="67">
         <v>3</v>
       </c>
-      <c r="N6" s="61">
-        <v>0</v>
-      </c>
-      <c r="O6" s="61">
+      <c r="N6" s="68">
+        <v>0</v>
+      </c>
+      <c r="O6" s="68">
         <v>73.27</v>
       </c>
-      <c r="P6" s="62">
-        <f t="shared" si="2"/>
+      <c r="P6" s="69">
         <v>73.27</v>
       </c>
-      <c r="Q6" s="61">
+      <c r="Q6" s="68">
         <v>17.760000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="60">
+      <c r="A7" s="67">
         <v>4</v>
       </c>
-      <c r="B7" s="61">
+      <c r="B7" s="68">
         <v>98.870249914412796</v>
       </c>
-      <c r="C7" s="61">
+      <c r="C7" s="68">
         <v>99.9</v>
       </c>
-      <c r="D7" s="62">
-        <f t="shared" si="0"/>
+      <c r="D7" s="69">
         <v>1.0297500855872102</v>
       </c>
-      <c r="E7" s="61">
+      <c r="E7" s="68">
         <v>97.13</v>
       </c>
-      <c r="G7" s="60">
+      <c r="F7" s="63"/>
+      <c r="G7" s="67">
         <v>4</v>
       </c>
-      <c r="H7" s="61">
+      <c r="H7" s="68">
         <v>98.778004073319707</v>
       </c>
-      <c r="I7" s="61">
+      <c r="I7" s="68">
         <v>99.389002036659804</v>
       </c>
-      <c r="J7" s="62">
-        <f t="shared" si="1"/>
+      <c r="J7" s="69">
         <v>0.61099796334009682</v>
       </c>
-      <c r="K7" s="61">
+      <c r="K7" s="68">
         <v>96.94</v>
       </c>
-      <c r="M7" s="60">
+      <c r="L7" s="63"/>
+      <c r="M7" s="67">
         <v>4</v>
       </c>
-      <c r="N7" s="61">
+      <c r="N7" s="68">
         <v>0.10183299389002</v>
       </c>
-      <c r="O7" s="61">
+      <c r="O7" s="68">
         <v>81.67</v>
       </c>
-      <c r="P7" s="62">
-        <f t="shared" si="2"/>
+      <c r="P7" s="69">
         <v>81.568167006109988</v>
       </c>
-      <c r="Q7" s="61">
+      <c r="Q7" s="68">
         <v>18.149999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="60">
+      <c r="A8" s="67">
         <v>5</v>
       </c>
-      <c r="B8" s="61">
+      <c r="B8" s="68">
         <v>98.985427042981001</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="68">
         <v>99.87</v>
       </c>
-      <c r="D8" s="62">
-        <f t="shared" si="0"/>
+      <c r="D8" s="69">
         <v>0.88457295701900307</v>
       </c>
-      <c r="E8" s="61">
+      <c r="E8" s="68">
         <v>89.79</v>
       </c>
-      <c r="G8" s="60">
+      <c r="F8" s="63"/>
+      <c r="G8" s="67">
         <v>5</v>
       </c>
-      <c r="H8" s="61">
+      <c r="H8" s="68">
         <v>98.654708520179298</v>
       </c>
-      <c r="I8" s="61">
+      <c r="I8" s="68">
         <v>99.22</v>
       </c>
-      <c r="J8" s="62">
-        <f t="shared" si="1"/>
+      <c r="J8" s="69">
         <v>0.56529147982070072</v>
       </c>
-      <c r="K8" s="61">
+      <c r="K8" s="68">
         <v>90.34</v>
       </c>
-      <c r="M8" s="60">
+      <c r="L8" s="63"/>
+      <c r="M8" s="67">
         <v>5</v>
       </c>
-      <c r="N8" s="61">
+      <c r="N8" s="68">
         <v>0.112107623318385</v>
       </c>
-      <c r="O8" s="61">
+      <c r="O8" s="68">
         <v>90.69</v>
       </c>
-      <c r="P8" s="62">
-        <f t="shared" si="2"/>
+      <c r="P8" s="69">
         <v>90.577892376681618</v>
       </c>
-      <c r="Q8" s="61">
+      <c r="Q8" s="68">
         <v>16.77</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="60">
+      <c r="A9" s="67">
         <v>6</v>
       </c>
-      <c r="B9" s="61">
+      <c r="B9" s="68">
         <v>99.036836769178706</v>
       </c>
-      <c r="C9" s="61">
+      <c r="C9" s="68">
         <v>99.97</v>
       </c>
-      <c r="D9" s="62">
-        <f t="shared" si="0"/>
+      <c r="D9" s="69">
         <v>0.93316323082129315</v>
       </c>
-      <c r="E9" s="61">
+      <c r="E9" s="68">
         <v>96.3</v>
       </c>
-      <c r="G9" s="60">
+      <c r="F9" s="63"/>
+      <c r="G9" s="67">
         <v>6</v>
       </c>
-      <c r="H9" s="61">
+      <c r="H9" s="68">
         <v>98.643006263047994</v>
       </c>
-      <c r="I9" s="61">
+      <c r="I9" s="68">
         <v>99.06</v>
       </c>
-      <c r="J9" s="62">
-        <f t="shared" si="1"/>
+      <c r="J9" s="69">
         <v>0.41699373695200848</v>
       </c>
-      <c r="K9" s="61">
+      <c r="K9" s="68">
         <v>95.71</v>
       </c>
-      <c r="M9" s="60">
+      <c r="L9" s="63"/>
+      <c r="M9" s="67">
         <v>6</v>
       </c>
-      <c r="N9" s="61">
+      <c r="N9" s="68">
         <v>0.73068893528183698</v>
       </c>
-      <c r="O9" s="61">
+      <c r="O9" s="68">
         <v>98.23</v>
       </c>
-      <c r="P9" s="62">
-        <f t="shared" si="2"/>
+      <c r="P9" s="69">
         <v>97.499311064718171</v>
       </c>
-      <c r="Q9" s="61">
+      <c r="Q9" s="68">
         <v>19.5</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="60">
+      <c r="A10" s="67">
         <v>8</v>
       </c>
-      <c r="B10" s="61">
+      <c r="B10" s="68">
         <v>99.025807554264205</v>
       </c>
-      <c r="C10" s="61">
+      <c r="C10" s="68">
         <v>99.88</v>
       </c>
-      <c r="D10" s="62">
-        <f t="shared" si="0"/>
+      <c r="D10" s="69">
         <v>0.85419244573579078</v>
       </c>
-      <c r="E10" s="61">
+      <c r="E10" s="68">
         <v>94.17</v>
       </c>
-      <c r="G10" s="60">
+      <c r="F10" s="63"/>
+      <c r="G10" s="67">
         <v>8</v>
       </c>
-      <c r="H10" s="61">
+      <c r="H10" s="68">
         <v>98.665297741273093</v>
       </c>
-      <c r="I10" s="61">
+      <c r="I10" s="68">
         <v>99.49</v>
       </c>
-      <c r="J10" s="62">
-        <f t="shared" si="1"/>
+      <c r="J10" s="69">
         <v>0.8247022587269015</v>
       </c>
-      <c r="K10" s="61">
+      <c r="K10" s="68">
         <v>93.47</v>
       </c>
-      <c r="M10" s="60">
+      <c r="L10" s="63"/>
+      <c r="M10" s="67">
         <v>8</v>
       </c>
-      <c r="N10" s="61">
-        <v>0</v>
-      </c>
-      <c r="O10" s="61">
+      <c r="N10" s="68">
+        <v>0</v>
+      </c>
+      <c r="O10" s="68">
         <v>63.55</v>
       </c>
-      <c r="P10" s="62">
-        <f t="shared" si="2"/>
+      <c r="P10" s="69">
         <v>63.55</v>
       </c>
-      <c r="Q10" s="61">
+      <c r="Q10" s="68">
         <v>16.5</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="60">
+      <c r="A11" s="67">
         <v>9</v>
       </c>
-      <c r="B11" s="61">
+      <c r="B11" s="68">
         <v>98.554378887207903</v>
       </c>
-      <c r="C11" s="61">
+      <c r="C11" s="68">
         <v>99.92</v>
       </c>
-      <c r="D11" s="62">
-        <f t="shared" si="0"/>
+      <c r="D11" s="69">
         <v>1.3656211127920983</v>
       </c>
-      <c r="E11" s="61">
+      <c r="E11" s="68">
         <v>96.54</v>
       </c>
-      <c r="G11" s="60">
+      <c r="F11" s="63"/>
+      <c r="G11" s="67">
         <v>9</v>
       </c>
-      <c r="H11" s="61">
+      <c r="H11" s="68">
         <v>97.224975222992995</v>
       </c>
-      <c r="I11" s="61">
+      <c r="I11" s="68">
         <v>98.71</v>
       </c>
-      <c r="J11" s="62">
-        <f t="shared" si="1"/>
+      <c r="J11" s="69">
         <v>1.4850247770069984</v>
       </c>
-      <c r="K11" s="61">
+      <c r="K11" s="68">
         <v>96.38</v>
       </c>
-      <c r="M11" s="60">
+      <c r="L11" s="63"/>
+      <c r="M11" s="67">
         <v>9</v>
       </c>
-      <c r="N11" s="61">
-        <v>0</v>
-      </c>
-      <c r="O11" s="61">
+      <c r="N11" s="68">
+        <v>0</v>
+      </c>
+      <c r="O11" s="68">
         <v>93.06</v>
       </c>
-      <c r="P11" s="62">
-        <f t="shared" si="2"/>
+      <c r="P11" s="69">
         <v>93.06</v>
       </c>
-      <c r="Q11" s="61">
+      <c r="Q11" s="68">
         <v>19.68</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="60">
+      <c r="B12" s="67">
         <v>98.99</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="G12" s="60" t="s">
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="60">
+      <c r="H12" s="67">
         <v>98.63</v>
       </c>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="M12" s="60" t="s">
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="N12" s="60">
+      <c r="N12" s="67">
         <v>10.38</v>
       </c>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="60"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72">
+        <v>96.48</v>
+      </c>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72">
+        <v>96.15</v>
+      </c>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="N13" s="72"/>
+      <c r="O13" s="72">
+        <v>29.73</v>
+      </c>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="67"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72">
+        <v>91.24</v>
+      </c>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" s="72"/>
+      <c r="I14" s="72">
+        <v>90.75</v>
+      </c>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="N14" s="72"/>
+      <c r="O14" s="72">
+        <v>62.94</v>
+      </c>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="67"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="72"/>
+      <c r="C15" s="72">
+        <v>91.65</v>
+      </c>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72">
+        <v>91.27</v>
+      </c>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="N15" s="72"/>
+      <c r="O15" s="72">
+        <v>57.85</v>
+      </c>
+      <c r="P15" s="67"/>
+      <c r="Q15" s="67"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72">
+        <v>95.18</v>
+      </c>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="72"/>
+      <c r="I16" s="72">
+        <v>94.39</v>
+      </c>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="N16" s="72"/>
+      <c r="O16" s="72">
+        <v>62.94</v>
+      </c>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67">
+        <v>91.65</v>
+      </c>
+      <c r="D17" s="73"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67">
+        <v>91.27</v>
+      </c>
+      <c r="J17" s="67"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="N17" s="72"/>
+      <c r="O17" s="72">
+        <v>57.85</v>
+      </c>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="67"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="70"/>
+      <c r="P18" s="71"/>
+      <c r="Q18" s="70"/>
+    </row>
+    <row r="19" spans="1:17" s="60" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="59">
-        <v>3836</v>
-      </c>
-      <c r="G15" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="K15" s="59">
-        <v>618</v>
-      </c>
-      <c r="M15" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="P15" s="59">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="59" t="s">
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="59">
-        <v>44181</v>
-      </c>
-      <c r="G16" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="K16" s="59">
-        <v>7426</v>
-      </c>
-      <c r="M16" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="P16" s="59">
-        <v>2830</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17" s="59">
-        <v>11983</v>
-      </c>
-      <c r="G17" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="K17" s="59">
-        <v>1956</v>
-      </c>
-      <c r="M17" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="P17" s="59">
-        <v>6011</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18" s="59">
-        <v>96.48</v>
-      </c>
-      <c r="D18"/>
-      <c r="G18" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="K18" s="59">
-        <v>96.15</v>
-      </c>
-      <c r="M18" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="P18" s="59">
-        <v>29.73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="64"/>
-      <c r="K19" s="64"/>
-      <c r="P19" s="64"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D20"/>
-      <c r="K20"/>
-      <c r="P20"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D21"/>
-      <c r="K21"/>
-      <c r="P21"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D22"/>
-      <c r="K22"/>
-      <c r="P22"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="63"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="65"/>
+      <c r="G20" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="63"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="67">
+        <v>0</v>
+      </c>
+      <c r="B21" s="67">
+        <v>98.92</v>
+      </c>
+      <c r="C21" s="67">
+        <v>99.93</v>
+      </c>
+      <c r="D21" s="69">
+        <v>1.0100000000000051</v>
+      </c>
+      <c r="E21" s="67">
+        <v>77.010000000000005</v>
+      </c>
+      <c r="F21" s="63"/>
+      <c r="G21" s="67">
+        <v>0</v>
+      </c>
+      <c r="H21" s="67">
+        <v>99.18</v>
+      </c>
+      <c r="I21" s="67">
+        <v>99.8</v>
+      </c>
+      <c r="J21" s="69">
+        <v>0.61999999999999034</v>
+      </c>
+      <c r="K21" s="67">
+        <v>77.78</v>
+      </c>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="63"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="67">
+        <v>1</v>
+      </c>
+      <c r="B22" s="67">
+        <v>97.92</v>
+      </c>
+      <c r="C22" s="67">
+        <v>99.64</v>
+      </c>
+      <c r="D22" s="69">
+        <v>1.7199999999999989</v>
+      </c>
+      <c r="E22" s="67">
+        <v>90</v>
+      </c>
+      <c r="F22" s="63"/>
+      <c r="G22" s="67">
+        <v>1</v>
+      </c>
+      <c r="H22" s="67">
+        <v>98.59</v>
+      </c>
+      <c r="I22" s="67">
+        <v>99.65</v>
+      </c>
+      <c r="J22" s="69">
+        <v>1.0600000000000023</v>
+      </c>
+      <c r="K22" s="67">
+        <v>90.25</v>
+      </c>
+      <c r="L22" s="63"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="63"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="67">
+        <v>2</v>
+      </c>
+      <c r="B23" s="67">
+        <v>97.78</v>
+      </c>
+      <c r="C23" s="67">
+        <v>96.24</v>
+      </c>
+      <c r="D23" s="69">
+        <v>-1.5400000000000063</v>
+      </c>
+      <c r="E23" s="67">
+        <v>75.61</v>
+      </c>
+      <c r="F23" s="63"/>
+      <c r="G23" s="67">
+        <v>2</v>
+      </c>
+      <c r="H23" s="67">
+        <v>97.29</v>
+      </c>
+      <c r="I23" s="67">
+        <v>95.16</v>
+      </c>
+      <c r="J23" s="69">
+        <v>-2.1300000000000097</v>
+      </c>
+      <c r="K23" s="67">
+        <v>76.02</v>
+      </c>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="67">
+        <v>3</v>
+      </c>
+      <c r="B24" s="67">
+        <v>95.84</v>
+      </c>
+      <c r="C24" s="67">
+        <v>99.15</v>
+      </c>
+      <c r="D24" s="69">
+        <v>3.3100000000000023</v>
+      </c>
+      <c r="E24" s="67">
+        <v>85.84</v>
+      </c>
+      <c r="F24" s="63"/>
+      <c r="G24" s="67">
+        <v>3</v>
+      </c>
+      <c r="H24" s="67">
+        <v>95.84</v>
+      </c>
+      <c r="I24" s="67">
+        <v>99.21</v>
+      </c>
+      <c r="J24" s="69">
+        <v>3.3699999999999903</v>
+      </c>
+      <c r="K24" s="67">
+        <v>85.47</v>
+      </c>
+      <c r="L24" s="63"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="63"/>
+      <c r="P24" s="63"/>
+      <c r="Q24" s="63"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="67">
+        <v>4</v>
+      </c>
+      <c r="B25" s="67">
+        <v>98.32</v>
+      </c>
+      <c r="C25" s="67">
+        <v>99.61</v>
+      </c>
+      <c r="D25" s="69">
+        <v>1.2900000000000063</v>
+      </c>
+      <c r="E25" s="67">
+        <v>94.25</v>
+      </c>
+      <c r="F25" s="63"/>
+      <c r="G25" s="67">
+        <v>4</v>
+      </c>
+      <c r="H25" s="67">
+        <v>98.37</v>
+      </c>
+      <c r="I25" s="67">
+        <v>99.59</v>
+      </c>
+      <c r="J25" s="69">
+        <v>1.2199999999999989</v>
+      </c>
+      <c r="K25" s="67">
+        <v>93.98</v>
+      </c>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="67">
+        <v>5</v>
+      </c>
+      <c r="B26" s="67">
+        <v>98.25</v>
+      </c>
+      <c r="C26" s="67">
+        <v>99.41</v>
+      </c>
+      <c r="D26" s="69">
+        <v>1.1599999999999966</v>
+      </c>
+      <c r="E26" s="67">
+        <v>86.12</v>
+      </c>
+      <c r="F26" s="63"/>
+      <c r="G26" s="67">
+        <v>5</v>
+      </c>
+      <c r="H26" s="67">
+        <v>98.99</v>
+      </c>
+      <c r="I26" s="67">
+        <v>99.78</v>
+      </c>
+      <c r="J26" s="69">
+        <v>0.79000000000000625</v>
+      </c>
+      <c r="K26" s="67">
+        <v>85.67</v>
+      </c>
+      <c r="L26" s="63"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="63"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="67">
+        <v>6</v>
+      </c>
+      <c r="B27" s="67">
+        <v>96.62</v>
+      </c>
+      <c r="C27" s="67">
+        <v>98.51</v>
+      </c>
+      <c r="D27" s="69">
+        <v>1.8900000000000006</v>
+      </c>
+      <c r="E27" s="67">
+        <v>96.6</v>
+      </c>
+      <c r="F27" s="63"/>
+      <c r="G27" s="67">
+        <v>6</v>
+      </c>
+      <c r="H27" s="67">
+        <v>95.72</v>
+      </c>
+      <c r="I27" s="67">
+        <v>97.91</v>
+      </c>
+      <c r="J27" s="69">
+        <v>2.1899999999999977</v>
+      </c>
+      <c r="K27" s="67">
+        <v>96.34</v>
+      </c>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="67">
+        <v>7</v>
+      </c>
+      <c r="B28" s="67">
+        <v>95.81</v>
+      </c>
+      <c r="C28" s="67">
+        <v>98.48</v>
+      </c>
+      <c r="D28" s="69">
+        <v>2.6700000000000017</v>
+      </c>
+      <c r="E28" s="67">
+        <v>95.75</v>
+      </c>
+      <c r="F28" s="63"/>
+      <c r="G28" s="67">
+        <v>7</v>
+      </c>
+      <c r="H28" s="67">
+        <v>94.74</v>
+      </c>
+      <c r="I28" s="67">
+        <v>98.35</v>
+      </c>
+      <c r="J28" s="69">
+        <v>3.6099999999999994</v>
+      </c>
+      <c r="K28" s="67">
+        <v>95.53</v>
+      </c>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="63"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="67">
+        <v>8</v>
+      </c>
+      <c r="B29" s="67">
+        <v>90.75</v>
+      </c>
+      <c r="C29" s="67">
+        <v>96.55</v>
+      </c>
+      <c r="D29" s="69">
+        <v>5.7999999999999972</v>
+      </c>
+      <c r="E29" s="67">
+        <v>95.48</v>
+      </c>
+      <c r="F29" s="63"/>
+      <c r="G29" s="67">
+        <v>7</v>
+      </c>
+      <c r="H29" s="67">
+        <v>89.63</v>
+      </c>
+      <c r="I29" s="67">
+        <v>96.1</v>
+      </c>
+      <c r="J29" s="69">
+        <v>6.4699999999999989</v>
+      </c>
+      <c r="K29" s="67">
+        <v>95.26</v>
+      </c>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="63"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="67">
+        <v>9</v>
+      </c>
+      <c r="B30" s="67">
+        <v>95.55</v>
+      </c>
+      <c r="C30" s="67">
+        <v>99.83</v>
+      </c>
+      <c r="D30" s="69">
+        <v>4.2800000000000011</v>
+      </c>
+      <c r="E30" s="67">
+        <v>73.62</v>
+      </c>
+      <c r="F30" s="63"/>
+      <c r="G30" s="67">
+        <v>9</v>
+      </c>
+      <c r="H30" s="67">
+        <v>94.95</v>
+      </c>
+      <c r="I30" s="67">
+        <v>99.6</v>
+      </c>
+      <c r="J30" s="69">
+        <v>4.6499999999999915</v>
+      </c>
+      <c r="K30" s="67">
+        <v>73.73</v>
+      </c>
+      <c r="L30" s="63"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="63"/>
+      <c r="P30" s="63"/>
+      <c r="Q30" s="63"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="67">
+        <v>96.58</v>
+      </c>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="H31" s="67">
+        <v>96.34</v>
+      </c>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="63"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="72"/>
+      <c r="C32" s="72">
+        <v>96.49</v>
+      </c>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72">
+        <v>96.31</v>
+      </c>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="63"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72">
+        <v>74.489999999999995</v>
+      </c>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72">
+        <v>74.31</v>
+      </c>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="K23"/>
-      <c r="P23"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="H24" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="I24" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="K24" s="46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="60">
-        <v>0</v>
-      </c>
-      <c r="B25" s="60">
-        <v>98.92</v>
-      </c>
-      <c r="C25" s="60">
-        <v>99.93</v>
-      </c>
-      <c r="D25" s="62">
-        <f>SUM(C25-B25)</f>
-        <v>1.0100000000000051</v>
-      </c>
-      <c r="E25" s="60">
-        <v>77.010000000000005</v>
-      </c>
-      <c r="G25" s="60">
-        <v>0</v>
-      </c>
-      <c r="H25" s="60">
-        <v>99.18</v>
-      </c>
-      <c r="I25" s="60">
-        <v>99.8</v>
-      </c>
-      <c r="J25" s="62">
-        <f>SUM(I25-H25)</f>
-        <v>0.61999999999999034</v>
-      </c>
-      <c r="K25" s="60">
-        <v>77.78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="60">
-        <v>1</v>
-      </c>
-      <c r="B26" s="60">
-        <v>97.92</v>
-      </c>
-      <c r="C26" s="60">
-        <v>99.64</v>
-      </c>
-      <c r="D26" s="62">
-        <f t="shared" ref="D26:D34" si="3">SUM(C26-B26)</f>
-        <v>1.7199999999999989</v>
-      </c>
-      <c r="E26" s="60">
-        <v>90</v>
-      </c>
-      <c r="G26" s="60">
-        <v>1</v>
-      </c>
-      <c r="H26" s="60">
-        <v>98.59</v>
-      </c>
-      <c r="I26" s="60">
-        <v>99.65</v>
-      </c>
-      <c r="J26" s="62">
-        <f t="shared" ref="J26:J34" si="4">SUM(I26-H26)</f>
-        <v>1.0600000000000023</v>
-      </c>
-      <c r="K26" s="60">
-        <v>90.25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="60">
-        <v>2</v>
-      </c>
-      <c r="B27" s="60">
-        <v>97.78</v>
-      </c>
-      <c r="C27" s="60">
-        <v>96.24</v>
-      </c>
-      <c r="D27" s="62">
-        <f t="shared" si="3"/>
-        <v>-1.5400000000000063</v>
-      </c>
-      <c r="E27" s="60">
-        <v>75.61</v>
-      </c>
-      <c r="G27" s="60">
-        <v>2</v>
-      </c>
-      <c r="H27" s="60">
-        <v>97.29</v>
-      </c>
-      <c r="I27" s="60">
-        <v>95.16</v>
-      </c>
-      <c r="J27" s="62">
-        <f t="shared" si="4"/>
-        <v>-2.1300000000000097</v>
-      </c>
-      <c r="K27" s="60">
-        <v>76.02</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="60">
-        <v>3</v>
-      </c>
-      <c r="B28" s="60">
-        <v>95.84</v>
-      </c>
-      <c r="C28" s="60">
-        <v>99.15</v>
-      </c>
-      <c r="D28" s="62">
-        <f t="shared" si="3"/>
-        <v>3.3100000000000023</v>
-      </c>
-      <c r="E28" s="60">
-        <v>85.84</v>
-      </c>
-      <c r="G28" s="60">
-        <v>3</v>
-      </c>
-      <c r="H28" s="60">
-        <v>95.84</v>
-      </c>
-      <c r="I28" s="60">
-        <v>99.21</v>
-      </c>
-      <c r="J28" s="62">
-        <f t="shared" si="4"/>
-        <v>3.3699999999999903</v>
-      </c>
-      <c r="K28" s="60">
-        <v>85.47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="60">
-        <v>4</v>
-      </c>
-      <c r="B29" s="60">
-        <v>98.32</v>
-      </c>
-      <c r="C29" s="60">
-        <v>99.61</v>
-      </c>
-      <c r="D29" s="62">
-        <f t="shared" si="3"/>
-        <v>1.2900000000000063</v>
-      </c>
-      <c r="E29" s="60">
-        <v>94.25</v>
-      </c>
-      <c r="G29" s="60">
-        <v>4</v>
-      </c>
-      <c r="H29" s="60">
-        <v>98.37</v>
-      </c>
-      <c r="I29" s="60">
-        <v>99.59</v>
-      </c>
-      <c r="J29" s="62">
-        <f t="shared" si="4"/>
-        <v>1.2199999999999989</v>
-      </c>
-      <c r="K29" s="60">
-        <v>93.98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="60">
-        <v>5</v>
-      </c>
-      <c r="B30" s="60">
-        <v>98.25</v>
-      </c>
-      <c r="C30" s="60">
-        <v>99.41</v>
-      </c>
-      <c r="D30" s="62">
-        <f t="shared" si="3"/>
-        <v>1.1599999999999966</v>
-      </c>
-      <c r="E30" s="60">
-        <v>86.12</v>
-      </c>
-      <c r="G30" s="60">
-        <v>5</v>
-      </c>
-      <c r="H30" s="60">
-        <v>98.99</v>
-      </c>
-      <c r="I30" s="60">
-        <v>99.78</v>
-      </c>
-      <c r="J30" s="62">
-        <f t="shared" si="4"/>
-        <v>0.79000000000000625</v>
-      </c>
-      <c r="K30" s="60">
-        <v>85.67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="60">
-        <v>6</v>
-      </c>
-      <c r="B31" s="60">
-        <v>96.62</v>
-      </c>
-      <c r="C31" s="60">
-        <v>98.51</v>
-      </c>
-      <c r="D31" s="62">
-        <f t="shared" si="3"/>
-        <v>1.8900000000000006</v>
-      </c>
-      <c r="E31" s="60">
-        <v>96.6</v>
-      </c>
-      <c r="G31" s="60">
-        <v>6</v>
-      </c>
-      <c r="H31" s="60">
-        <v>95.72</v>
-      </c>
-      <c r="I31" s="60">
-        <v>97.91</v>
-      </c>
-      <c r="J31" s="62">
-        <f t="shared" si="4"/>
-        <v>2.1899999999999977</v>
-      </c>
-      <c r="K31" s="60">
-        <v>96.34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="60">
-        <v>7</v>
-      </c>
-      <c r="B32" s="60">
-        <v>95.81</v>
-      </c>
-      <c r="C32" s="60">
-        <v>98.48</v>
-      </c>
-      <c r="D32" s="62">
-        <f t="shared" si="3"/>
-        <v>2.6700000000000017</v>
-      </c>
-      <c r="E32" s="60">
-        <v>95.75</v>
-      </c>
-      <c r="G32" s="60">
-        <v>7</v>
-      </c>
-      <c r="H32" s="60">
-        <v>94.74</v>
-      </c>
-      <c r="I32" s="60">
-        <v>98.35</v>
-      </c>
-      <c r="J32" s="62">
-        <f t="shared" si="4"/>
-        <v>3.6099999999999994</v>
-      </c>
-      <c r="K32" s="60">
-        <v>95.53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="60">
-        <v>8</v>
-      </c>
-      <c r="B33" s="60">
-        <v>90.75</v>
-      </c>
-      <c r="C33" s="60">
-        <v>96.55</v>
-      </c>
-      <c r="D33" s="62">
-        <f t="shared" si="3"/>
-        <v>5.7999999999999972</v>
-      </c>
-      <c r="E33" s="60">
-        <v>95.48</v>
-      </c>
-      <c r="G33" s="60">
-        <v>8</v>
-      </c>
-      <c r="H33" s="60">
-        <v>89.63</v>
-      </c>
-      <c r="I33" s="60">
-        <v>96.1</v>
-      </c>
-      <c r="J33" s="62">
-        <f t="shared" si="4"/>
-        <v>6.4699999999999989</v>
-      </c>
-      <c r="K33" s="60">
-        <v>95.26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="60">
-        <v>9</v>
-      </c>
-      <c r="B34" s="60">
-        <v>95.55</v>
-      </c>
-      <c r="C34" s="60">
-        <v>99.83</v>
-      </c>
-      <c r="D34" s="62">
-        <f t="shared" si="3"/>
-        <v>4.2800000000000011</v>
-      </c>
-      <c r="E34" s="60">
-        <v>73.62</v>
-      </c>
-      <c r="G34" s="60">
-        <v>9</v>
-      </c>
-      <c r="H34" s="60">
-        <v>94.95</v>
-      </c>
-      <c r="I34" s="60">
-        <v>99.6</v>
-      </c>
-      <c r="J34" s="62">
-        <f t="shared" si="4"/>
-        <v>4.6499999999999915</v>
-      </c>
-      <c r="K34" s="60">
-        <v>73.73</v>
-      </c>
+      <c r="B34" s="72"/>
+      <c r="C34" s="72">
+        <v>79.959999999999994</v>
+      </c>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72">
+        <v>80.069999999999993</v>
+      </c>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="60">
-        <v>96.58</v>
-      </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="G35" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="H35" s="60">
-        <v>96.34</v>
-      </c>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="60"/>
+      <c r="A35" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72">
+        <v>90.28</v>
+      </c>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" s="72"/>
+      <c r="I35" s="72">
+        <v>90.48</v>
+      </c>
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="67"/>
+      <c r="C36" s="67">
+        <v>84.82</v>
+      </c>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="67"/>
+      <c r="I36" s="67">
+        <v>85.34</v>
+      </c>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8604,22 +8883,22 @@
         <v>93</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -8941,17 +9220,17 @@
       <c r="A5" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="65" t="s">
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="66"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="54"/>
@@ -9035,17 +9314,17 @@
       <c r="A9" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="65" t="s">
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="66"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="54"/>
@@ -9249,17 +9528,17 @@
       <c r="A20" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="65" t="s">
+      <c r="B20" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="65" t="s">
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="H20" s="66"/>
+      <c r="H20" s="62"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="54" t="s">
@@ -9323,17 +9602,17 @@
       <c r="A24" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="65" t="s">
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="H24" s="66"/>
+      <c r="H24" s="62"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="54"/>

</xml_diff>